<commit_message>
New modified columns added, time to figure out how to update modified content
</commit_message>
<xml_diff>
--- a/MergedResults.xlsx
+++ b/MergedResults.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="13">
   <si>
     <t>User</t>
   </si>
@@ -26,6 +26,18 @@
   </si>
   <si>
     <t>Is Z Done?</t>
+  </si>
+  <si>
+    <t>User-Modified</t>
+  </si>
+  <si>
+    <t>Is X Done?-Modified</t>
+  </si>
+  <si>
+    <t>Is Y done?-Modified</t>
+  </si>
+  <si>
+    <t>Is Z Done?-Modified</t>
   </si>
   <si>
     <t>Created Date</t>
@@ -376,7 +388,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E18"/>
+  <dimension ref="A1:I18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -384,7 +396,7 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:9">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -400,294 +412,306 @@
       <c r="E1" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="2" spans="1:5">
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9">
       <c r="A2" t="n">
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="C2" t="s">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="D2" t="s">
-        <v>5</v>
-      </c>
-      <c r="E2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5">
+        <v>9</v>
+      </c>
+      <c r="I2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9">
       <c r="A3" t="n">
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="C3" t="s">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="D3" t="s">
-        <v>5</v>
-      </c>
-      <c r="E3" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5">
+        <v>9</v>
+      </c>
+      <c r="I3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9">
       <c r="A4" t="n">
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="C4" t="s">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="D4" t="s">
-        <v>5</v>
-      </c>
-      <c r="E4" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5">
+        <v>9</v>
+      </c>
+      <c r="I4" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9">
       <c r="A5" t="n">
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="C5" t="s">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="D5" t="s">
-        <v>5</v>
-      </c>
-      <c r="E5" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5">
+        <v>9</v>
+      </c>
+      <c r="I5" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9">
       <c r="A6" t="n">
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="C6" t="s">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="D6" t="s">
-        <v>5</v>
-      </c>
-      <c r="E6" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5">
+        <v>9</v>
+      </c>
+      <c r="I6" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9">
       <c r="A7" t="n">
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="C7" t="s">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="D7" t="s">
-        <v>5</v>
-      </c>
-      <c r="E7" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5">
+        <v>9</v>
+      </c>
+      <c r="I7" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9">
       <c r="A8" t="n">
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="C8" t="s">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="D8" t="s">
-        <v>5</v>
-      </c>
-      <c r="E8" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5">
+        <v>9</v>
+      </c>
+      <c r="I8" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9">
       <c r="A9" t="n">
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="C9" t="s">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="D9" t="s">
-        <v>5</v>
-      </c>
-      <c r="E9" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5">
+        <v>9</v>
+      </c>
+      <c r="I9" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9">
       <c r="A10" t="n">
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="C10" t="s">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="D10" t="s">
-        <v>5</v>
-      </c>
-      <c r="E10" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5">
+        <v>9</v>
+      </c>
+      <c r="I10" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9">
       <c r="A11" t="n">
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="C11" t="s">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="D11" t="s">
-        <v>5</v>
-      </c>
-      <c r="E11" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5">
+        <v>9</v>
+      </c>
+      <c r="I11" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9">
       <c r="A12" t="n">
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="C12" t="s">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="D12" t="s">
-        <v>5</v>
-      </c>
-      <c r="E12" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5">
+        <v>9</v>
+      </c>
+      <c r="I12" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9">
       <c r="A13" t="n">
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="C13" t="s">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="D13" t="s">
-        <v>5</v>
-      </c>
-      <c r="E13" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5">
+        <v>9</v>
+      </c>
+      <c r="I13" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9">
       <c r="A14" t="n">
         <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="C14" t="s">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="D14" t="s">
-        <v>5</v>
-      </c>
-      <c r="E14" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5">
+        <v>9</v>
+      </c>
+      <c r="I14" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9">
       <c r="A15" t="n">
         <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="C15" t="s">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="D15" t="s">
-        <v>5</v>
-      </c>
-      <c r="E15" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5">
+        <v>9</v>
+      </c>
+      <c r="I15" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9">
       <c r="A16" t="n">
         <v>15</v>
       </c>
       <c r="B16" t="s">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="C16" t="s">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="D16" t="s">
-        <v>5</v>
-      </c>
-      <c r="E16" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5">
+        <v>9</v>
+      </c>
+      <c r="I16" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9">
       <c r="A17" t="n">
         <v>16</v>
       </c>
       <c r="B17" t="s">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="C17" t="s">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="D17" t="s">
-        <v>7</v>
-      </c>
-      <c r="E17" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5">
+        <v>11</v>
+      </c>
+      <c r="I17" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9">
       <c r="A18" t="n">
         <v>17</v>
       </c>
       <c r="B18" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="C18" t="s">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="D18" t="s">
-        <v>5</v>
-      </c>
-      <c r="E18" t="s">
-        <v>8</v>
+        <v>9</v>
+      </c>
+      <c r="I18" t="s">
+        <v>12</v>
       </c>
     </row>
   </sheetData>

</xml_diff>